<commit_message>
Testing related modifications for tag improvment
</commit_message>
<xml_diff>
--- a/wordlist/wordlist.xlsx
+++ b/wordlist/wordlist.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\web_scraping_cursos\web_scraping\web-scraping-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chistopherholder/Desktop/FirmenABC_scraper/outreach_automation/wordlist/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892B4480-6AC3-8146-BA01-19524B2629B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="3920" yWindow="1840" windowWidth="23040" windowHeight="9200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -59,9 +60,6 @@
     <t>Karriere</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Zurzeit keine offenen Stellen</t>
   </si>
   <si>
@@ -77,9 +75,6 @@
     <t>Keine offenen</t>
   </si>
   <si>
-    <t>Maybe</t>
-  </si>
-  <si>
     <t>Initiativ</t>
   </si>
   <si>
@@ -95,9 +90,6 @@
     <t>Initiativbewerbung</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Freie Stellen</t>
   </si>
   <si>
@@ -107,9 +99,6 @@
     <t>auf der Suche</t>
   </si>
   <si>
-    <t>Fuck Yes</t>
-  </si>
-  <si>
     <t xml:space="preserve"> ab sofort</t>
   </si>
   <si>
@@ -135,12 +124,24 @@
   </si>
   <si>
     <t>Aktuell auf der Suche</t>
+  </si>
+  <si>
+    <t>NoHire</t>
+  </si>
+  <si>
+    <t>MaybeHire</t>
+  </si>
+  <si>
+    <t>YesHire</t>
+  </si>
+  <si>
+    <t>HireNow</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -474,20 +475,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
     <col min="2" max="2" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -495,7 +496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -503,7 +504,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -511,7 +512,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -519,7 +520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -527,7 +528,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -535,7 +536,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -543,7 +544,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -551,7 +552,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -559,212 +560,212 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="2" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="2" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="2" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="2" t="s">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" s="2" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="2" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="2" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" s="2" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>